<commit_message>
20230420 update: update test case.
</commit_message>
<xml_diff>
--- a/TestData/TestCase.xlsx
+++ b/TestData/TestCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codegen\OutResult\Cloud\NET.SDK\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells.cloud-sdk-node\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D9AD0C-6B08-4085-83D6-136989B7FC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B156701A-FAA1-4E48-BE30-BAFD44B28F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_Sheet1C5E131" hidden="1">Sheet1!$C$5:$E$13</definedName>
+    <definedName name="_xlcn.WorksheetConnection_Sheet1C5E13" hidden="1">Sheet1!$C$5:$E$13</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
-    <pivotCache cacheId="7" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -56,7 +56,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range-d213b4da-b744-44db-ac10-bdbf77e88844" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1C5E131"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_Sheet1C5E13"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Id</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>(All)</t>
   </si>
 </sst>
 </file>
@@ -328,10 +331,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisPage" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -373,20 +376,12 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="0" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Count" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
@@ -403,7 +398,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D2E2DBAA-4DE7-4C0F-8B0C-C5F3597E2F3D}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D2E2DBAA-4DE7-4C0F-8B0C-C5F3597E2F3D}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -413,7 +408,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" measureFilter="1">
       <items count="6">
         <item x="0"/>
         <item x="2"/>
@@ -437,6 +432,9 @@
   </rowFields>
   <rowItems count="5">
     <i>
+      <x/>
+    </i>
+    <i>
       <x v="1"/>
     </i>
     <i>
@@ -444,9 +442,6 @@
     </i>
     <i>
       <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -471,11 +466,11 @@
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <filters count="1">
-    <filter fld="1" type="captionGreaterThan" evalOrder="-1" id="1" stringValue1="3">
+    <filter fld="1" type="valueNotEqual" evalOrder="-1" id="2" iMeasureFld="0">
       <autoFilter ref="A1">
         <filterColumn colId="0">
           <customFilters>
-            <customFilter operator="greaterThan" val="3"/>
+            <customFilter operator="notEqual" val="0"/>
           </customFilters>
         </filterColumn>
       </autoFilter>
@@ -493,7 +488,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -963,6 +958,50 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{7AB02ACF-6CA4-4BF7-963D-3CFB18FFCC18}">
+          <x14:colorSeries rgb="FF323232"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!E6:E6</xm:f>
+              <xm:sqref>I6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E7:E7</xm:f>
+              <xm:sqref>I7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E8:E8</xm:f>
+              <xm:sqref>I8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E9:E9</xm:f>
+              <xm:sqref>I9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E10:E10</xm:f>
+              <xm:sqref>I10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E11:E11</xm:f>
+              <xm:sqref>I11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E12:E12</xm:f>
+              <xm:sqref>I12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!E13:E13</xm:f>
+              <xm:sqref>I13</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{46DF9E0D-C88D-4997-BC4E-6E53B7ED24C1}">
           <x14:colorSeries rgb="FF323232"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -1007,50 +1046,6 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{7AB02ACF-6CA4-4BF7-963D-3CFB18FFCC18}">
-          <x14:colorSeries rgb="FF323232"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!E6:E6</xm:f>
-              <xm:sqref>I6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!E7:E7</xm:f>
-              <xm:sqref>I7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!E8:E8</xm:f>
-              <xm:sqref>I8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!E9:E9</xm:f>
-              <xm:sqref>I9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!E10:E10</xm:f>
-              <xm:sqref>I10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!E11:E11</xm:f>
-              <xm:sqref>I11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!E12:E12</xm:f>
-              <xm:sqref>I12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!E13:E13</xm:f>
-              <xm:sqref>I13</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
@@ -1059,114 +1054,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:D10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A3:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
       <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="B9" s="3">
         <v>29</v>
       </c>
     </row>
@@ -1179,17 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07B6ADE-1516-46BE-B85B-A2DBCED674DE}">
   <dimension ref="A3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" start="4" max="6" activeRow="8" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" fieldPosition="0">
-          <references count="1">
-            <reference field="1" count="1">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,50 +1178,50 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3">
+        <v>7</v>
+      </c>
       <c r="D7" s="3">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1275,13 +1229,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3">
         <v>7</v>
       </c>
       <c r="D9" s="3">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>